<commit_message>
Added tutorials.js Added menu.js ------------ Version 1.0
</commit_message>
<xml_diff>
--- a/TM/resources/data/config/data.xlsx
+++ b/TM/resources/data/config/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c815833208247f46/IdeaProjects/TM/TM/resources/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{DEC2DE00-B768-403F-8438-3D29A38DA369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D43D8F97-0E11-40F4-9B22-6C85ED76FC89}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{DEC2DE00-B768-403F-8438-3D29A38DA369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36CC5392-0B99-450A-824C-E3D13494A58A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A969FF00-14EC-47C5-8179-A132855C2957}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="216">
   <si>
     <t>ID</t>
   </si>
@@ -71,12 +71,6 @@
     <t>Es-tu fatigué?</t>
   </si>
   <si>
-    <t xml:space="preserve">Veux tu te coucher? </t>
-  </si>
-  <si>
-    <t>Veux tu un verre d'eau?</t>
-  </si>
-  <si>
     <t>As-tu besoin de te moucher?</t>
   </si>
   <si>
@@ -104,12 +98,6 @@
     <t>Ton copain veut pas jouer avec toi?</t>
   </si>
   <si>
-    <t>Un copain a prit un de tes jouets?</t>
-  </si>
-  <si>
-    <t>Un copain a prit le jeu avec lequel tu voulais jouer?</t>
-  </si>
-  <si>
     <t>Qui?</t>
   </si>
   <si>
@@ -119,12 +107,6 @@
     <t>Tu peux attendre?</t>
   </si>
   <si>
-    <t>Attend 5 minutes.</t>
-  </si>
-  <si>
-    <t>Attend la pause.</t>
-  </si>
-  <si>
     <t>Tu peux y aller.</t>
   </si>
   <si>
@@ -140,9 +122,6 @@
     <t>Reste avec moi pendant la pause.</t>
   </si>
   <si>
-    <t>Tu n'as pas comprit ce qu'il fallait faire?</t>
-  </si>
-  <si>
     <t>Tu veux colorier?</t>
   </si>
   <si>
@@ -305,12 +284,6 @@
     <t>${camarades} ("ne veut pas" | "n'as pas envie" | "refuse" | "n'est pas d'accord" | "n'as pas voulu") "jouer avec toi?"</t>
   </si>
   <si>
-    <t>${camarades} ("a prit" | "t'as piqué" | "t'as volé") ("un de tes" | "ton") "jouet?"</t>
-  </si>
-  <si>
-    <t>${camarades} ("a prit" | "t'as piqué" | "t'as volé") ("un des" | "le") "jouet?" ("avec lequel tu" ("voulais jouer" | "jouais"))? "?"</t>
-  </si>
-  <si>
     <t>"c'est"? "qui" "qui as fait ça"? "?"</t>
   </si>
   <si>
@@ -323,9 +296,6 @@
     <t>"Vas-y."</t>
   </si>
   <si>
-    <t>"Attend la pause." | "Pas tout de suite."</t>
-  </si>
-  <si>
     <t>${ne-pas-pouvoir} ("attendre" | "patienter") ("un petit moment" | "5 minutes")? "?"</t>
   </si>
   <si>
@@ -338,21 +308,9 @@
     <t>"Attend" ("5 minutes" | ("encore"? "un moment")) "."</t>
   </si>
   <si>
-    <t>${avoir-besoin} "qu'un" ${camarades} ("t'accompagne?" | "viennes avec toi?")</t>
-  </si>
-  <si>
-    <t>"c'est"? "pas grave."</t>
-  </si>
-  <si>
-    <t>"On va" "te"? "trouver" ("des" | "une") "nouveau"? "propre"? ("culotte" | "vêtements" | "habits" | "slip") "."</t>
-  </si>
-  <si>
     <t>"Reste avec moi pendant la pause"</t>
   </si>
   <si>
-    <t>${avoir-interrogatif} "comprit" ("ce qu'il fallait faire" | "la consigne") "?"</t>
-  </si>
-  <si>
     <t>("Veux-tu" | "Tu-veux") ("colorier" | "faire un coloriage" | "faire un dessin") "?"</t>
   </si>
   <si>
@@ -377,36 +335,21 @@
     <t>"Tu n'y arrives pas?"</t>
   </si>
   <si>
-    <t>("C'est où que" | "Où") ("as-tu" | "tu as")  "mal?"</t>
-  </si>
-  <si>
     <t>("C'est quand que t'as bu" | "Quand est ce que tu as bu") "pour la dernière fois"? "?"</t>
   </si>
   <si>
     <t>"Tu as oublié tes affaires de gym?"</t>
   </si>
   <si>
-    <t>"Je vais t'en prêter"</t>
-  </si>
-  <si>
-    <t>"Ne t'inquiète pas."</t>
-  </si>
-  <si>
     <t>("c'est"? "pas un problème.") | "Aucun problème." | "pas de problème"</t>
   </si>
   <si>
     <t>"Tu veux que je vienne" "avec toi"? ("voir" | "regarder")? "?"</t>
   </si>
   <si>
-    <t>"Tu n'a pas" ("pensé à prendre" | "pris") "tes" ("affaires" | "habits") "de" ("sports" | "gym") "?"</t>
-  </si>
-  <si>
     <t>"Tu as" ("regardé" | "vérifié") "dans ton" ("cartable" | "sac") "?"</t>
   </si>
   <si>
-    <t>"Ne t'inquiète pas,"? "je vais" ("t'en" ("prêter" | "passer" | "donner" | "trouver") | "te ("prêter" | "passer" | "donner" | "trouver") ("des affaires" | "des habits" ("de sport" | "de gym"))) "?"</t>
-  </si>
-  <si>
     <t>"C'est pas grave,"? "tu feras la gym comme" ("ça" | "tu es" | "sans")</t>
   </si>
   <si>
@@ -431,9 +374,6 @@
     <t>${avoir-besoin} ("t'asseoir" | "venir") "un moment"? "sur mes genoux?"</t>
   </si>
   <si>
-    <t>"Tu les" ("retrouveras" | "reveras") "(tout"? "bientôt." | "tout à l'heure" | "dans peu de temps")</t>
-  </si>
-  <si>
     <t>Was tut dir weh?</t>
   </si>
   <si>
@@ -614,15 +554,9 @@
     <t>Toilette</t>
   </si>
   <si>
-    <t>Est-ce que tu dois aller aux Toilette?</t>
-  </si>
-  <si>
     <t>${avoir-besoin} ("aller aux Toilette?" | "faire pipi?")</t>
   </si>
   <si>
-    <t>"Tu peux" "y"? "aller" "aux Toilette"? "."</t>
-  </si>
-  <si>
     <t>Verstehen</t>
   </si>
   <si>
@@ -654,6 +588,102 @@
   </si>
   <si>
     <t>Il faut que tu boives quelque chose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veux-tu te coucher? </t>
+  </si>
+  <si>
+    <t>Veux-tu un verre d'eau?</t>
+  </si>
+  <si>
+    <t>Un copain a pris un de tes jouets?</t>
+  </si>
+  <si>
+    <t>Un copain a pris le jeu avec lequel tu voulais jouer?</t>
+  </si>
+  <si>
+    <t>${camarades} ("a pris" | "t'as piqué" | "t'as volé") ("un de tes" | "ton") "jouet?"</t>
+  </si>
+  <si>
+    <t>${camarades} ("a pris" | "t'as piqué" | "t'as volé") ("un des" | "le") "jouet?" ("avec lequel tu" ("voulais jouer" | "jouais"))? "?"</t>
+  </si>
+  <si>
+    <t>Tu n'as pas compris ce qu'il fallait faire?</t>
+  </si>
+  <si>
+    <t>${avoir-interrogatif} "compris" ("ce qu'il fallait faire" | "la consigne") "?"</t>
+  </si>
+  <si>
+    <t>Est-ce que tu dois aller aux toilettes?</t>
+  </si>
+  <si>
+    <t>Attends la pause.</t>
+  </si>
+  <si>
+    <t>Attends 5 minutes.</t>
+  </si>
+  <si>
+    <t>("C'est où que tu as" | "Où as-tu")  "mal?"</t>
+  </si>
+  <si>
+    <t>("C'est où que tu t'es" | "Où t'es-tu")  "blessé?"</t>
+  </si>
+  <si>
+    <t>"Tu peux" "y"? "aller" "aux toilette"? "."</t>
+  </si>
+  <si>
+    <t>"Attends la pause." | "Pas tout de suite."</t>
+  </si>
+  <si>
+    <t>${avoir-besoin} "qu'un" ${camarades} ("t'accompagne?" | "vienne avec toi?")</t>
+  </si>
+  <si>
+    <t>"Tu n'as pas" ("pensé à prendre" | "pris") "tes" ("affaires" | "habits") "de" ("sports" | "gym") "?"</t>
+  </si>
+  <si>
+    <t>("Es-tu" | "Tu es") ("en colère" | "fâché") ("contre" ${camarades})? "?"</t>
+  </si>
+  <si>
+    <t>("Es-tu" | "Tu es") "effrayé"</t>
+  </si>
+  <si>
+    <t>("As-tu" | "Tu as") ("peur" | "la trouille") "sans tes parents"? "?"</t>
+  </si>
+  <si>
+    <t>("Es-tu" | "Tu es") "triste?"</t>
+  </si>
+  <si>
+    <t>${avoir-interrogatif} "des démangeaisons?"</t>
+  </si>
+  <si>
+    <t>"est-ce que"? "ça te" ("gratte" | "démange") "?"</t>
+  </si>
+  <si>
+    <t>("As-tu" | "Tu as") ("perdu" | "égaré") ("quelque chose" | "ton doudou" | "ton dessin" | "ta trousse")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"On va" "te"? "trouver" ("des" | "une") "nouveau"? "propre"? ("culotte" | "vêtements" | "habits" | "slip") ${pas-inquietude}? "." </t>
+  </si>
+  <si>
+    <t>"viens"? "on va" "tout"? ("nettoyer" | "laver") ("tout"? "ça") ${pas-inquietude}?</t>
+  </si>
+  <si>
+    <t>("Respire" | "Inspire" "expire"?) ("calmement" | "tranquillement" | "doucement")? ${pas-inquietude}?</t>
+  </si>
+  <si>
+    <t>${pas-inquietude}</t>
+  </si>
+  <si>
+    <t>"Je vais t'en prêter" ${pas-inquietude}?</t>
+  </si>
+  <si>
+    <t>${pas-inquietude}? "je vais" ("t'en" ("prêter" | "passer" | "donner" | "trouver") | "te ("prêter" | "passer" | "donner" | "trouver") ("des affaires" | "des habits" ("de sport" | "de gym"))) "?"</t>
+  </si>
+  <si>
+    <t>("C'est pas grave" | "C'est pas un problème") ${pas-inquietude}?</t>
+  </si>
+  <si>
+    <t>"Tu les" ("retrouveras" | "reveras") "(tout"? "bientôt." | "tout à l'heure" | "dans peu de temps") ${pas-inquietude}?</t>
   </si>
 </sst>
 </file>
@@ -689,8 +719,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,8 +746,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{391721AE-C6F8-40CE-A59C-4E389E90C2CE}" name="source" displayName="source" ref="A1:E66" totalsRowShown="0">
   <autoFilter ref="A1:E66" xr:uid="{391721AE-C6F8-40CE-A59C-4E389E90C2CE}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E53">
-    <sortCondition ref="A1:A53"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E66">
+    <sortCondition ref="A1:A66"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{1716B642-98D8-4295-BFFE-663EDA72A024}" name="ID"/>
@@ -730,10 +761,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{50C567AC-8E16-4000-A514-575847E8D5AA}" name="variants" displayName="variants" ref="H1:J71" totalsRowShown="0">
-  <autoFilter ref="H1:J71" xr:uid="{50C567AC-8E16-4000-A514-575847E8D5AA}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:J29">
-    <sortCondition ref="H1:H29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{50C567AC-8E16-4000-A514-575847E8D5AA}" name="variants" displayName="variants" ref="H1:J81" totalsRowShown="0">
+  <autoFilter ref="H1:J81" xr:uid="{50C567AC-8E16-4000-A514-575847E8D5AA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:J73">
+    <sortCondition ref="H1:H73"/>
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{251A51FB-719E-42FE-95F5-982121B6294A}" name="ID"/>
@@ -1063,10 +1094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FE23BE-6B97-4336-80D7-C2BD76844489}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="83" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="E46" zoomScale="83" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,7 +1128,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -1106,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1117,13 +1148,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -1133,7 +1164,7 @@
         <v>Où as-tu mal?</v>
       </c>
       <c r="J2" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1141,26 +1172,26 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="str">
         <f>VLOOKUP(H3,source[],4)</f>
-        <v>Montre-moi.</v>
+        <v>Où as-tu mal?</v>
       </c>
       <c r="J3" t="s">
-        <v>55</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1171,23 +1202,23 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" t="str">
         <f>VLOOKUP(H4,source[],4)</f>
-        <v>C'est un copain qui t'as fait ça?</v>
+        <v>Montre-moi.</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1198,23 +1229,23 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I5" t="str">
         <f>VLOOKUP(H5,source[],4)</f>
-        <v>As-tu faim?</v>
+        <v>C'est un copain qui t'as fait ça?</v>
       </c>
       <c r="J5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1225,13 +1256,13 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>135</v>
+        <v>115</v>
       </c>
       <c r="H6">
         <v>3</v>
@@ -1241,7 +1272,7 @@
         <v>As-tu faim?</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1252,23 +1283,23 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I7" t="str">
         <f>VLOOKUP(H7,source[],4)</f>
-        <v>As-tu besoin de vomir?</v>
+        <v>As-tu faim?</v>
       </c>
       <c r="J7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1279,23 +1310,23 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>138</v>
+        <v>118</v>
       </c>
       <c r="H8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8" t="str">
         <f>VLOOKUP(H8,source[],4)</f>
-        <v>Quelqu'un t'as tapé?</v>
+        <v>As-tu besoin de vomir?</v>
       </c>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1306,23 +1337,23 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="H9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I9" t="str">
         <f>VLOOKUP(H9,source[],4)</f>
-        <v>Quand est-ce que tu as bu pour la dernière fois?</v>
+        <v>Quelqu'un t'as tapé?</v>
       </c>
       <c r="J9" t="s">
-        <v>114</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1333,13 +1364,13 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>184</v>
       </c>
       <c r="E10" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="H10">
         <v>6</v>
@@ -1349,7 +1380,7 @@
         <v>Quand est-ce que tu as bu pour la dernière fois?</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1360,13 +1391,13 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
       <c r="H11">
         <v>6</v>
@@ -1376,7 +1407,7 @@
         <v>Quand est-ce que tu as bu pour la dernière fois?</v>
       </c>
       <c r="J11" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1387,23 +1418,23 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="H12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I12" t="str">
         <f>VLOOKUP(H12,source[],4)</f>
-        <v>Es-tu fatigué?</v>
+        <v>Quand est-ce que tu as bu pour la dernière fois?</v>
       </c>
       <c r="J12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1414,13 +1445,13 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>185</v>
       </c>
       <c r="E13" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
       <c r="H13">
         <v>7</v>
@@ -1430,7 +1461,7 @@
         <v>Es-tu fatigué?</v>
       </c>
       <c r="J13" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1441,23 +1472,23 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
       <c r="H14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I14" t="str">
         <f>VLOOKUP(H14,source[],4)</f>
-        <v xml:space="preserve">Veux tu te coucher? </v>
+        <v>Es-tu fatigué?</v>
       </c>
       <c r="J14" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1468,23 +1499,23 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="H15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I15" t="str">
         <f>VLOOKUP(H15,source[],4)</f>
-        <v>Veux-tu t'asseoir un moment?</v>
+        <v xml:space="preserve">Veux-tu te coucher? </v>
       </c>
       <c r="J15" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1495,23 +1526,23 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="H16">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I16" t="str">
         <f>VLOOKUP(H16,source[],4)</f>
-        <v>Veux-tu t'asseoir un moment avec un doudou?</v>
+        <v>Veux-tu t'asseoir un moment?</v>
       </c>
       <c r="J16" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1522,23 +1553,23 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="H17">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I17" t="str">
         <f>VLOOKUP(H17,source[],4)</f>
-        <v>Veux tu un verre d'eau?</v>
+        <v>Veux-tu t'asseoir un moment avec un doudou?</v>
       </c>
       <c r="J17" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1546,26 +1577,26 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="H18">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I18" t="str">
         <f>VLOOKUP(H18,source[],4)</f>
-        <v>As-tu besoin de te moucher?</v>
+        <v>Veux-tu un verre d'eau?</v>
       </c>
       <c r="J18" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1576,23 +1607,23 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="H19">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I19" t="str">
         <f>VLOOKUP(H19,source[],4)</f>
-        <v>As-tu froid?</v>
+        <v>As-tu besoin de te moucher?</v>
       </c>
       <c r="J19" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1603,23 +1634,23 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D20" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="H20">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I20" t="str">
         <f>VLOOKUP(H20,source[],4)</f>
-        <v>As-tu chaud?</v>
+        <v>As-tu froid?</v>
       </c>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1630,23 +1661,23 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="H21">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I21" t="str">
         <f>VLOOKUP(H21,source[],4)</f>
-        <v>Veux-tu enlever ton pull?</v>
+        <v>As-tu chaud?</v>
       </c>
       <c r="J21" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -1657,23 +1688,23 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="H22">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I22" t="str">
         <f>VLOOKUP(H22,source[],4)</f>
-        <v>On va mettre ta main sous l'eau.</v>
+        <v>Veux-tu enlever ton pull?</v>
       </c>
       <c r="J22" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1684,23 +1715,23 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="H23">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I23" t="str">
         <f>VLOOKUP(H23,source[],4)</f>
-        <v>Tu as mal au pied?</v>
+        <v>On va mettre ta main sous l'eau.</v>
       </c>
       <c r="J23" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1711,23 +1742,23 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="H24">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I24" t="str">
         <f>VLOOKUP(H24,source[],4)</f>
-        <v>Tu as mal à la jambe?</v>
+        <v>Tu as mal au pied?</v>
       </c>
       <c r="J24" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -1738,23 +1769,23 @@
         <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="H25">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I25" t="str">
         <f>VLOOKUP(H25,source[],4)</f>
-        <v>Tu as mal au bras?</v>
+        <v>Tu as mal à la jambe?</v>
       </c>
       <c r="J25" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -1765,23 +1796,23 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="H26">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I26" t="str">
         <f>VLOOKUP(H26,source[],4)</f>
-        <v>Tu as mal à la tête?</v>
+        <v>Tu as mal au bras?</v>
       </c>
       <c r="J26" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -1792,23 +1823,23 @@
         <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>186</v>
       </c>
       <c r="E27" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="H27">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I27" t="str">
         <f>VLOOKUP(H27,source[],4)</f>
-        <v>Tu as mal au ventre?</v>
+        <v>Tu as mal à la tête?</v>
       </c>
       <c r="J27" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -1819,23 +1850,23 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D28" t="s">
-        <v>23</v>
+        <v>187</v>
       </c>
       <c r="E28" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="H28">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I28" t="str">
         <f>VLOOKUP(H28,source[],4)</f>
-        <v>Tu as mal à la gorge?</v>
+        <v>Tu as mal au ventre?</v>
       </c>
       <c r="J28" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -1846,23 +1877,23 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E29" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="H29">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I29" t="str">
         <f>VLOOKUP(H29,source[],4)</f>
-        <v>Ici?</v>
+        <v>Tu as mal à la gorge?</v>
       </c>
       <c r="J29" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -1873,23 +1904,23 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D30" t="s">
         <v>192</v>
       </c>
       <c r="E30" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="H30">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I30" t="str">
         <f>VLOOKUP(H30,source[],4)</f>
-        <v>Ton copain veut pas jouer avec toi?</v>
+        <v>Ici?</v>
       </c>
       <c r="J30" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -1900,23 +1931,23 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="H31">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I31" t="str">
         <f>VLOOKUP(H31,source[],4)</f>
-        <v>Un copain a prit un de tes jouets?</v>
+        <v>Ton copain veut pas jouer avec toi?</v>
       </c>
       <c r="J31" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -1924,26 +1955,26 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D32" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="H32">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I32" t="str">
         <f>VLOOKUP(H32,source[],4)</f>
-        <v>Un copain a prit le jeu avec lequel tu voulais jouer?</v>
+        <v>Un copain a pris un de tes jouets?</v>
       </c>
       <c r="J32" t="s">
-        <v>90</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -1951,26 +1982,26 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>193</v>
       </c>
       <c r="E33" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="H33">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I33" t="str">
         <f>VLOOKUP(H33,source[],4)</f>
-        <v>Qui?</v>
+        <v>Un copain a pris le jeu avec lequel tu voulais jouer?</v>
       </c>
       <c r="J33" t="s">
-        <v>91</v>
+        <v>189</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -1981,13 +2012,13 @@
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D34" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="H34">
         <v>27</v>
@@ -1997,7 +2028,7 @@
         <v>Qui?</v>
       </c>
       <c r="J34" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -2005,26 +2036,26 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D35" t="s">
+        <v>194</v>
+      </c>
+      <c r="E35" t="s">
+        <v>144</v>
+      </c>
+      <c r="H35">
         <v>27</v>
-      </c>
-      <c r="E35" t="s">
-        <v>164</v>
-      </c>
-      <c r="H35">
-        <v>28</v>
       </c>
       <c r="I35" t="str">
         <f>VLOOKUP(H35,source[],4)</f>
-        <v>Est-ce que tu dois aller aux Toilette?</v>
+        <v>Qui?</v>
       </c>
       <c r="J35" t="s">
-        <v>193</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -2035,23 +2066,23 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E36" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="H36">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I36" t="str">
         <f>VLOOKUP(H36,source[],4)</f>
-        <v>Est-ce que tu t'es fait pipi dessus?</v>
+        <v>Est-ce que tu dois aller aux toilettes?</v>
       </c>
       <c r="J36" t="s">
-        <v>93</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -2059,26 +2090,26 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E37" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="H37">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I37" t="str">
         <f>VLOOKUP(H37,source[],4)</f>
-        <v>Tu peux y aller.</v>
+        <v>Est-ce que tu t'es fait pipi dessus?</v>
       </c>
       <c r="J37" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -2086,16 +2117,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D38" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E38" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="H38">
         <v>30</v>
@@ -2105,7 +2136,7 @@
         <v>Tu peux y aller.</v>
       </c>
       <c r="J38" t="s">
-        <v>194</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -2113,26 +2144,26 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E39" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="H39">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I39" t="str">
         <f>VLOOKUP(H39,source[],4)</f>
-        <v>Attend la pause.</v>
+        <v>Tu peux y aller.</v>
       </c>
       <c r="J39" t="s">
-        <v>95</v>
+        <v>197</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -2143,23 +2174,23 @@
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
+        <v>190</v>
       </c>
       <c r="E40" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="H40">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I40" t="str">
         <f>VLOOKUP(H40,source[],4)</f>
-        <v>Tu peux attendre?</v>
+        <v>Attends la pause.</v>
       </c>
       <c r="J40" t="s">
-        <v>96</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
@@ -2170,13 +2201,13 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D41" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E41" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="H41">
         <v>32</v>
@@ -2186,7 +2217,7 @@
         <v>Tu peux attendre?</v>
       </c>
       <c r="J41" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -2197,23 +2228,23 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D42" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E42" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="H42">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I42" t="str">
         <f>VLOOKUP(H42,source[],4)</f>
-        <v>Attend 5 minutes.</v>
+        <v>Tu peux attendre?</v>
       </c>
       <c r="J42" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
@@ -2224,23 +2255,23 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E43" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="H43">
         <v>33</v>
       </c>
       <c r="I43" t="str">
         <f>VLOOKUP(H43,source[],4)</f>
-        <v>Attend 5 minutes.</v>
+        <v>Attends 5 minutes.</v>
       </c>
       <c r="J43" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
@@ -2251,23 +2282,23 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D44" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E44" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="H44">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I44" t="str">
         <f>VLOOKUP(H44,source[],4)</f>
-        <v>Tu veux qu'un copain t'accompagne?</v>
+        <v>Attends 5 minutes.</v>
       </c>
       <c r="J44" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
@@ -2278,23 +2309,23 @@
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D45" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E45" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="H45">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I45" t="str">
         <f>VLOOKUP(H45,source[],4)</f>
-        <v>C'est pas grave</v>
+        <v>Tu veux qu'un copain t'accompagne?</v>
       </c>
       <c r="J45" t="s">
-        <v>101</v>
+        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
@@ -2305,13 +2336,13 @@
         <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D46" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E46" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="H46">
         <v>35</v>
@@ -2321,7 +2352,7 @@
         <v>C'est pas grave</v>
       </c>
       <c r="J46" t="s">
-        <v>118</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
@@ -2332,23 +2363,23 @@
         <v>4</v>
       </c>
       <c r="C47" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D47" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E47" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="H47">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I47" t="str">
         <f>VLOOKUP(H47,source[],4)</f>
-        <v>On va te trouver des nouveaux vêtements</v>
+        <v>C'est pas grave</v>
       </c>
       <c r="J47" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
@@ -2359,23 +2390,23 @@
         <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D48" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E48" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="H48">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I48" t="str">
         <f>VLOOKUP(H48,source[],4)</f>
-        <v>Reste avec moi pendant la pause.</v>
+        <v>On va te trouver des nouveaux vêtements</v>
       </c>
       <c r="J48" t="s">
-        <v>103</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
@@ -2383,26 +2414,26 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D49" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E49" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="H49">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I49" t="str">
         <f>VLOOKUP(H49,source[],4)</f>
-        <v>Tu n'as pas comprit ce qu'il fallait faire?</v>
+        <v>Reste avec moi pendant la pause.</v>
       </c>
       <c r="J49" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
@@ -2410,26 +2441,26 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D50" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E50" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="H50">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I50" t="str">
         <f>VLOOKUP(H50,source[],4)</f>
-        <v>Tu veux colorier?</v>
+        <v>Tu n'as pas compris ce qu'il fallait faire?</v>
       </c>
       <c r="J50" t="s">
-        <v>105</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
@@ -2440,23 +2471,23 @@
         <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E51" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="H51">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I51" t="str">
         <f>VLOOKUP(H51,source[],4)</f>
-        <v>Tu veux prendre quelque chose dans ton sac?</v>
+        <v>Tu veux colorier?</v>
       </c>
       <c r="J51" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
@@ -2467,23 +2498,23 @@
         <v>4</v>
       </c>
       <c r="C52" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D52" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E52" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="H52">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I52" t="str">
         <f>VLOOKUP(H52,source[],4)</f>
-        <v>Un doudou?</v>
+        <v>Tu veux prendre quelque chose dans ton sac?</v>
       </c>
       <c r="J52" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
@@ -2491,16 +2522,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D53" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E53" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="H53">
         <v>41</v>
@@ -2510,7 +2541,7 @@
         <v>Un doudou?</v>
       </c>
       <c r="J53" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
@@ -2521,23 +2552,23 @@
         <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D54" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="E54" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="H54">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I54" t="str">
         <f>VLOOKUP(H54,source[],4)</f>
-        <v>Tu as besoin d'aide?</v>
+        <v>Un doudou?</v>
       </c>
       <c r="J54" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
@@ -2548,23 +2579,23 @@
         <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D55" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E55" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="H55">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I55" t="str">
         <f>VLOOKUP(H55,source[],4)</f>
-        <v>Tu n'y arrives pas?</v>
+        <v>Tu as besoin d'aide?</v>
       </c>
       <c r="J55" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
@@ -2575,23 +2606,23 @@
         <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D56" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E56" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="H56">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I56" t="str">
         <f>VLOOKUP(H56,source[],4)</f>
-        <v>Tu veux que je vienne voir?</v>
+        <v>Tu n'y arrives pas?</v>
       </c>
       <c r="J56" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
@@ -2602,23 +2633,23 @@
         <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D57" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E57" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="H57">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I57" t="str">
         <f>VLOOKUP(H57,source[],4)</f>
-        <v>Tu as oublié tes affaires de gym?</v>
+        <v>Tu veux que je vienne voir?</v>
       </c>
       <c r="J57" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
@@ -2626,26 +2657,26 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="D58" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E58" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="H58">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I58" t="str">
         <f>VLOOKUP(H58,source[],4)</f>
-        <v>Tu as regardé dans ton sac?</v>
+        <v>Tu as oublié tes affaires de gym?</v>
       </c>
       <c r="J58" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
@@ -2656,20 +2687,20 @@
         <v>4</v>
       </c>
       <c r="C59" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="D59" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="H59">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I59" t="str">
         <f>VLOOKUP(H59,source[],4)</f>
-        <v>Je vais t'en prêter</v>
+        <v>Tu as oublié tes affaires de gym?</v>
       </c>
       <c r="J59" t="s">
-        <v>116</v>
+        <v>200</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
@@ -2680,20 +2711,20 @@
         <v>4</v>
       </c>
       <c r="C60" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="D60" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="H60">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I60" t="str">
         <f>VLOOKUP(H60,source[],4)</f>
-        <v>C'est pas grave, tu feras la gym comme ça</v>
+        <v>Tu as regardé dans ton sac?</v>
       </c>
       <c r="J60" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
@@ -2704,20 +2735,20 @@
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="D61" t="s">
-        <v>200</v>
+        <v>178</v>
       </c>
       <c r="H61">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I61" t="str">
         <f>VLOOKUP(H61,source[],4)</f>
-        <v>Tu as un problème avec ton dessin?</v>
+        <v>Je vais t'en prêter</v>
       </c>
       <c r="J61" t="s">
-        <v>124</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -2728,20 +2759,20 @@
         <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D62" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="H62">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I62" t="str">
         <f>VLOOKUP(H62,source[],4)</f>
-        <v>Tes parents te manquent?</v>
+        <v>Je vais t'en prêter</v>
       </c>
       <c r="J62" t="s">
-        <v>125</v>
+        <v>213</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
@@ -2752,20 +2783,20 @@
         <v>4</v>
       </c>
       <c r="C63" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="D63" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="H63">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I63" t="str">
         <f>VLOOKUP(H63,source[],4)</f>
-        <v>Ne t'inquiète pas.</v>
+        <v>C'est pas grave, tu feras la gym comme ça</v>
       </c>
       <c r="J63" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
@@ -2773,23 +2804,23 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C64" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="D64" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="H64">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="I64" t="str">
         <f>VLOOKUP(H64,source[],4)</f>
-        <v>Veux-tu rester un moment tranquillement avec moi?</v>
+        <v>Tu as un problème avec ton dessin?</v>
       </c>
       <c r="J64" t="s">
-        <v>127</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
@@ -2797,23 +2828,23 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C65" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="D65" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="H65">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I65" t="str">
         <f>VLOOKUP(H65,source[],4)</f>
-        <v>Veux-tu rester un moment avec moi avec un livre?</v>
+        <v>Tes parents te manquent?</v>
       </c>
       <c r="J65" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
@@ -2821,83 +2852,203 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C66" t="s">
-        <v>189</v>
-      </c>
-      <c r="D66" t="s">
-        <v>205</v>
+        <v>169</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="H66">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I66" t="str">
         <f>VLOOKUP(H66,source[],4)</f>
-        <v>Veux-tu un doudou?</v>
+        <v>Tes parents te manquent?</v>
       </c>
       <c r="J66" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H67">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I67" t="str">
         <f>VLOOKUP(H67,source[],4)</f>
-        <v>Veux-tu t'asseoir sur mes genoux?</v>
+        <v>Ne t'inquiète pas.</v>
       </c>
       <c r="J67" t="s">
-        <v>130</v>
+        <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H68">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I68" t="str">
         <f>VLOOKUP(H68,source[],4)</f>
-        <v>Tu les retrouveras tout bientôt.</v>
+        <v>Veux-tu rester un moment tranquillement avec moi?</v>
       </c>
       <c r="J68" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H69">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="I69" t="str">
         <f>VLOOKUP(H69,source[],4)</f>
-        <v>Tu as oublié tes affaires de gym?</v>
+        <v>Veux-tu rester un moment avec moi avec un livre?</v>
       </c>
       <c r="J69" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H70">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I70" t="str">
         <f>VLOOKUP(H70,source[],4)</f>
-        <v>Je vais t'en prêter</v>
+        <v>Veux-tu un doudou?</v>
       </c>
       <c r="J70" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H71">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="I71" t="str">
         <f>VLOOKUP(H71,source[],4)</f>
-        <v>Tes parents te manquent?</v>
+        <v>Veux-tu t'asseoir sur mes genoux?</v>
       </c>
       <c r="J71" t="s">
-        <v>126</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H72">
+        <v>56</v>
+      </c>
+      <c r="I72" t="str">
+        <f>VLOOKUP(H72,source[],4)</f>
+        <v>Tu les retrouveras tout bientôt.</v>
+      </c>
+      <c r="J72" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H73">
+        <v>57</v>
+      </c>
+      <c r="I73" t="str">
+        <f>VLOOKUP(H73,source[],4)</f>
+        <v>Es-tu en colère?</v>
+      </c>
+      <c r="J73" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H74">
+        <v>58</v>
+      </c>
+      <c r="I74" t="str">
+        <f>VLOOKUP(H74,source[],4)</f>
+        <v>As-tu peur?</v>
+      </c>
+      <c r="J74" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H75">
+        <v>58</v>
+      </c>
+      <c r="I75" t="str">
+        <f>VLOOKUP(H75,source[],4)</f>
+        <v>As-tu peur?</v>
+      </c>
+      <c r="J75" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H76">
+        <v>59</v>
+      </c>
+      <c r="I76" t="str">
+        <f>VLOOKUP(H76,source[],4)</f>
+        <v>Es-tu triste?</v>
+      </c>
+      <c r="J76" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H77">
+        <v>60</v>
+      </c>
+      <c r="I77" t="str">
+        <f>VLOOKUP(H77,source[],4)</f>
+        <v>As-tu des démangeaisons ?</v>
+      </c>
+      <c r="J77" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H78">
+        <v>60</v>
+      </c>
+      <c r="I78" t="str">
+        <f>VLOOKUP(H78,source[],4)</f>
+        <v>As-tu des démangeaisons ?</v>
+      </c>
+      <c r="J78" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H79">
+        <v>61</v>
+      </c>
+      <c r="I79" t="str">
+        <f>VLOOKUP(H79,source[],4)</f>
+        <v>As-tu perdu quelque chose ?</v>
+      </c>
+      <c r="J79" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H80">
+        <v>62</v>
+      </c>
+      <c r="I80" t="str">
+        <f>VLOOKUP(H80,source[],4)</f>
+        <v>On va nettoyer ça, ne t’inquiète pas.</v>
+      </c>
+      <c r="J80" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="81" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H81">
+        <v>63</v>
+      </c>
+      <c r="I81" t="str">
+        <f>VLOOKUP(H81,source[],4)</f>
+        <v>Respire calmement, ça va passer.</v>
+      </c>
+      <c r="J81" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2910,6 +3061,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5e3a48d8-7e97-4140-96a4-9af8ed81797d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D0C1FCA18A99D34AAFDDFF46DD1E91A1" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e541d088f59b4fc9f823a894c4e813a1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5e3a48d8-7e97-4140-96a4-9af8ed81797d" xmlns:ns4="5f85ec69-15ba-4716-b649-82af49937962" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="291725a629dd727e9cbbb438f4c55961" ns3:_="" ns4:_="">
     <xsd:import namespace="5e3a48d8-7e97-4140-96a4-9af8ed81797d"/>
@@ -3130,38 +3298,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5e3a48d8-7e97-4140-96a4-9af8ed81797d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1210E72-E394-4977-A48D-DF6B50442432}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0838CF8F-8378-4A1D-A58E-CCAEB0AEECC0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="5e3a48d8-7e97-4140-96a4-9af8ed81797d"/>
-    <ds:schemaRef ds:uri="5f85ec69-15ba-4716-b649-82af49937962"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3184,9 +3324,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0838CF8F-8378-4A1D-A58E-CCAEB0AEECC0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1210E72-E394-4977-A48D-DF6B50442432}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="5e3a48d8-7e97-4140-96a4-9af8ed81797d"/>
+    <ds:schemaRef ds:uri="5f85ec69-15ba-4716-b649-82af49937962"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added about.html ------------ Version 1.1
</commit_message>
<xml_diff>
--- a/TM/resources/data/config/data.xlsx
+++ b/TM/resources/data/config/data.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c815833208247f46/IdeaProjects/TM/TM/resources/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="8_{DEC2DE00-B768-403F-8438-3D29A38DA369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36CC5392-0B99-450A-824C-E3D13494A58A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70C894FD-3F37-4833-8D80-651A37B72941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{A969FF00-14EC-47C5-8179-A132855C2957}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="233">
   <si>
     <t>ID</t>
   </si>
@@ -449,12 +449,6 @@
     <t>Will dein Freund nicht mit dir spielen?</t>
   </si>
   <si>
-    <t>Hat ein Kamarad dein Spielzeug weggenommen?</t>
-  </si>
-  <si>
-    <t>Hat ein Kamarad das Spielzeug weggenommen, mit dem du spielen wolltest?</t>
-  </si>
-  <si>
     <t>Wer war das?</t>
   </si>
   <si>
@@ -575,9 +569,6 @@
     <t>Es-tu triste?</t>
   </si>
   <si>
-    <t>As-tu des démangeaisons ?</t>
-  </si>
-  <si>
     <t>As-tu perdu quelque chose ?</t>
   </si>
   <si>
@@ -684,6 +675,66 @@
   </si>
   <si>
     <t>"Tu les" ("retrouveras" | "reveras") "(tout"? "bientôt." | "tout à l'heure" | "dans peu de temps") ${pas-inquietude}?</t>
+  </si>
+  <si>
+    <t>Hast du Angst?</t>
+  </si>
+  <si>
+    <t>Bist du traurig?</t>
+  </si>
+  <si>
+    <t>Hast du etwas verloren?</t>
+  </si>
+  <si>
+    <t>Hat ein Kamerad dein Spielzeug weggenommen?</t>
+  </si>
+  <si>
+    <t>Hat ein Kamerad das Spielzeug weggenommen, mit dem du spielen wolltest?</t>
+  </si>
+  <si>
+    <t>Tu as perdu quelque chose?</t>
+  </si>
+  <si>
+    <t>Tu veux me montrer quelque chose?</t>
+  </si>
+  <si>
+    <t>("je vais" | "on va") ("te trouver" | "te chercher") ("un verre d'eau" | "un truc à boire" | "quelque chose à boire") "?"</t>
+  </si>
+  <si>
+    <t>${pas-inquietude} ("il faut que tu boives" | "il faudrait que tu boives" | "tu dois boire" | "tu devrais boire") ("quelque chose" | "un truc" | "de l'eau" | "un verre d'eau")? "?"</t>
+  </si>
+  <si>
+    <t>"tu as perdu" ("quelque chose" | "un truc") "?"</t>
+  </si>
+  <si>
+    <t>"tu cherches" ("quelque chose" | "un truc") "?"</t>
+  </si>
+  <si>
+    <t>${avoir-besoin} "montrer" ("quelque chose" | "un truc") "?"</t>
+  </si>
+  <si>
+    <t>(${avoir-interrogatif} | "il y a") ("quelque chose" | "un truc") "que" ${avoir-besoin} "me montrer?"</t>
+  </si>
+  <si>
+    <t>Ça te gratte quelque part?</t>
+  </si>
+  <si>
+    <t>Mach dir keine Sorgen, das machen wir wieder sauber!</t>
+  </si>
+  <si>
+    <t>Du musst dringend etwas trinken.</t>
+  </si>
+  <si>
+    <t>Willst du mir etwas zeigen?</t>
+  </si>
+  <si>
+    <t>Bist du wütend?</t>
+  </si>
+  <si>
+    <t>Juckt es dich irgendwo?</t>
+  </si>
+  <si>
+    <t>Atme ruhig, es wird alles gut.</t>
   </si>
 </sst>
 </file>
@@ -707,7 +758,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -715,18 +766,235 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -739,30 +1007,26 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{391721AE-C6F8-40CE-A59C-4E389E90C2CE}" name="source" displayName="source" ref="A1:E66" totalsRowShown="0">
-  <autoFilter ref="A1:E66" xr:uid="{391721AE-C6F8-40CE-A59C-4E389E90C2CE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{391721AE-C6F8-40CE-A59C-4E389E90C2CE}" name="source" displayName="source" ref="A1:E68" totalsRowShown="0" tableBorderDxfId="5">
+  <autoFilter ref="A1:E68" xr:uid="{391721AE-C6F8-40CE-A59C-4E389E90C2CE}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E66">
     <sortCondition ref="A1:A66"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{1716B642-98D8-4295-BFFE-663EDA72A024}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{940FBD0D-E1F7-4F8D-B8DE-9DABC26859F3}" name="Type"/>
-    <tableColumn id="3" xr3:uid="{C97E8189-6F28-4423-A22D-BE23268817F2}" name="Theme"/>
-    <tableColumn id="4" xr3:uid="{16C5F967-ADBE-47C7-8F8D-36A8134F5918}" name="Phrase"/>
-    <tableColumn id="5" xr3:uid="{90FF2082-2B8F-428C-B75F-8073A68A1A72}" name="DE"/>
+    <tableColumn id="1" xr3:uid="{1716B642-98D8-4295-BFFE-663EDA72A024}" name="ID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{940FBD0D-E1F7-4F8D-B8DE-9DABC26859F3}" name="Type" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{C97E8189-6F28-4423-A22D-BE23268817F2}" name="Theme" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{16C5F967-ADBE-47C7-8F8D-36A8134F5918}" name="Phrase" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{90FF2082-2B8F-428C-B75F-8073A68A1A72}" name="DE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{50C567AC-8E16-4000-A514-575847E8D5AA}" name="variants" displayName="variants" ref="H1:J81" totalsRowShown="0">
-  <autoFilter ref="H1:J81" xr:uid="{50C567AC-8E16-4000-A514-575847E8D5AA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{50C567AC-8E16-4000-A514-575847E8D5AA}" name="variants" displayName="variants" ref="H1:J87" totalsRowShown="0">
+  <autoFilter ref="H1:J87" xr:uid="{50C567AC-8E16-4000-A514-575847E8D5AA}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:J73">
     <sortCondition ref="H1:H73"/>
   </sortState>
@@ -1094,21 +1358,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FE23BE-6B97-4336-80D7-C2BD76844489}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E46" zoomScale="83" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="46.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.88671875" customWidth="1"/>
     <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="9" max="9" width="43.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="153.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="149.44140625" customWidth="1"/>
     <col min="11" max="11" width="16.21875" customWidth="1"/>
     <col min="12" max="12" width="9.5546875" customWidth="1"/>
     <col min="13" max="13" width="15.109375" customWidth="1"/>
@@ -1141,19 +1406,19 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>112</v>
       </c>
       <c r="H2">
@@ -1164,23 +1429,23 @@
         <v>Où as-tu mal?</v>
       </c>
       <c r="J2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>116</v>
       </c>
       <c r="H3">
@@ -1191,23 +1456,23 @@
         <v>Où as-tu mal?</v>
       </c>
       <c r="J3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>113</v>
       </c>
       <c r="H4">
@@ -1222,19 +1487,19 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>169</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>114</v>
       </c>
       <c r="H5">
@@ -1249,19 +1514,19 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>169</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>115</v>
       </c>
       <c r="H6">
@@ -1276,19 +1541,19 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>117</v>
       </c>
       <c r="H7">
@@ -1303,19 +1568,19 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>169</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>118</v>
       </c>
       <c r="H8">
@@ -1330,19 +1595,19 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>169</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>119</v>
       </c>
       <c r="H9">
@@ -1357,19 +1622,19 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>169</v>
-      </c>
-      <c r="D10" t="s">
-        <v>184</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>120</v>
       </c>
       <c r="H10">
@@ -1384,19 +1649,19 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>169</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>121</v>
       </c>
       <c r="H11">
@@ -1411,19 +1676,19 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>169</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>122</v>
       </c>
       <c r="H12">
@@ -1438,19 +1703,19 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="2">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>169</v>
-      </c>
-      <c r="D13" t="s">
-        <v>185</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>123</v>
       </c>
       <c r="H13">
@@ -1465,19 +1730,19 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="2">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>169</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>124</v>
       </c>
       <c r="H14">
@@ -1492,19 +1757,19 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="2">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>169</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>125</v>
       </c>
       <c r="H15">
@@ -1519,19 +1784,19 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="2">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>169</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>126</v>
       </c>
       <c r="H16">
@@ -1546,19 +1811,19 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="2">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>169</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="3" t="s">
         <v>127</v>
       </c>
       <c r="H17">
@@ -1573,19 +1838,19 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="2">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C18" t="s">
-        <v>169</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="3" t="s">
         <v>128</v>
       </c>
       <c r="H18">
@@ -1600,19 +1865,19 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="2">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>169</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="3" t="s">
         <v>129</v>
       </c>
       <c r="H19">
@@ -1627,19 +1892,19 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="2">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" t="s">
-        <v>169</v>
-      </c>
-      <c r="D20" t="s">
+      <c r="B20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="3" t="s">
         <v>130</v>
       </c>
       <c r="H20">
@@ -1654,19 +1919,19 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="2">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>169</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="B21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="3" t="s">
         <v>131</v>
       </c>
       <c r="H21">
@@ -1681,19 +1946,19 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="2">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>169</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="3" t="s">
         <v>132</v>
       </c>
       <c r="H22">
@@ -1708,19 +1973,19 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="2">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="B23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="3" t="s">
         <v>133</v>
       </c>
       <c r="H23">
@@ -1735,19 +2000,19 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="2">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>169</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="B24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="3" t="s">
         <v>134</v>
       </c>
       <c r="H24">
@@ -1762,19 +2027,19 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="2">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>169</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="B25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="3" t="s">
         <v>135</v>
       </c>
       <c r="H25">
@@ -1789,19 +2054,19 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="2">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" t="s">
-        <v>170</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="B26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="3" t="s">
         <v>136</v>
       </c>
       <c r="H26">
@@ -1816,20 +2081,20 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="2">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" t="s">
-        <v>186</v>
-      </c>
-      <c r="E27" t="s">
-        <v>137</v>
+      <c r="B27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>216</v>
       </c>
       <c r="H27">
         <v>20</v>
@@ -1843,20 +2108,20 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="2">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>170</v>
-      </c>
-      <c r="D28" t="s">
-        <v>187</v>
-      </c>
-      <c r="E28" t="s">
-        <v>138</v>
+      <c r="B28" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>217</v>
       </c>
       <c r="H28">
         <v>21</v>
@@ -1870,20 +2135,20 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="2">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>170</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="B29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E29" t="s">
-        <v>139</v>
+      <c r="E29" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="H29">
         <v>22</v>
@@ -1897,20 +2162,20 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="2">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>171</v>
-      </c>
-      <c r="D30" t="s">
-        <v>192</v>
-      </c>
-      <c r="E30" t="s">
-        <v>140</v>
+      <c r="B30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="H30">
         <v>23</v>
@@ -1924,20 +2189,20 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="2">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>171</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="B31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E31" t="s">
-        <v>141</v>
+      <c r="E31" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="H31">
         <v>24</v>
@@ -1951,20 +2216,20 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32">
+      <c r="A32" s="2">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C32" t="s">
-        <v>171</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="C32" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E32" t="s">
-        <v>142</v>
+      <c r="E32" s="3" t="s">
+        <v>140</v>
       </c>
       <c r="H32">
         <v>25</v>
@@ -1974,24 +2239,24 @@
         <v>Un copain a pris un de tes jouets?</v>
       </c>
       <c r="J32" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33">
+      <c r="A33" s="2">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C33" t="s">
-        <v>171</v>
-      </c>
-      <c r="D33" t="s">
-        <v>193</v>
-      </c>
-      <c r="E33" t="s">
-        <v>145</v>
+      <c r="C33" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="H33">
         <v>26</v>
@@ -2001,24 +2266,24 @@
         <v>Un copain a pris le jeu avec lequel tu voulais jouer?</v>
       </c>
       <c r="J33" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="A34" s="2">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>171</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="B34" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E34" t="s">
-        <v>143</v>
+      <c r="E34" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="H34">
         <v>27</v>
@@ -2032,20 +2297,20 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="2">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C35" t="s">
-        <v>171</v>
-      </c>
-      <c r="D35" t="s">
-        <v>194</v>
-      </c>
-      <c r="E35" t="s">
-        <v>144</v>
+      <c r="C35" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="H35">
         <v>27</v>
@@ -2059,20 +2324,20 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="2">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>171</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="B36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E36" t="s">
-        <v>146</v>
+      <c r="E36" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="H36">
         <v>28</v>
@@ -2082,24 +2347,24 @@
         <v>Est-ce que tu dois aller aux toilettes?</v>
       </c>
       <c r="J36" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A37" s="2">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C37" t="s">
-        <v>171</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="C37" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E37" t="s">
-        <v>147</v>
+      <c r="E37" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="H37">
         <v>29</v>
@@ -2113,20 +2378,20 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="A38" s="2">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C38" t="s">
-        <v>171</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="C38" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E38" t="s">
-        <v>148</v>
+      <c r="E38" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="H38">
         <v>30</v>
@@ -2140,20 +2405,20 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39">
+      <c r="A39" s="2">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C39" t="s">
-        <v>171</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="C39" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E39" t="s">
-        <v>149</v>
+      <c r="E39" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="H39">
         <v>30</v>
@@ -2163,24 +2428,24 @@
         <v>Tu peux y aller.</v>
       </c>
       <c r="J39" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40">
+      <c r="A40" s="2">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>173</v>
-      </c>
-      <c r="D40" t="s">
-        <v>190</v>
-      </c>
-      <c r="E40" t="s">
-        <v>150</v>
+      <c r="B40" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="H40">
         <v>31</v>
@@ -2190,24 +2455,24 @@
         <v>Attends la pause.</v>
       </c>
       <c r="J40" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="A41" s="2">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" t="s">
-        <v>173</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="B41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E41" t="s">
-        <v>151</v>
+      <c r="E41" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="H41">
         <v>32</v>
@@ -2221,20 +2486,20 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="A42" s="2">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" t="s">
-        <v>173</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="B42" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E42" t="s">
-        <v>152</v>
+      <c r="E42" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="H42">
         <v>32</v>
@@ -2248,20 +2513,20 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="A43" s="2">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>173</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="B43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E43" t="s">
-        <v>153</v>
+      <c r="E43" s="3" t="s">
+        <v>151</v>
       </c>
       <c r="H43">
         <v>33</v>
@@ -2275,20 +2540,20 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44">
+      <c r="A44" s="2">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" t="s">
-        <v>173</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="B44" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E44" t="s">
-        <v>154</v>
+      <c r="E44" s="3" t="s">
+        <v>152</v>
       </c>
       <c r="H44">
         <v>33</v>
@@ -2302,20 +2567,20 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45">
+      <c r="A45" s="2">
         <v>43</v>
       </c>
-      <c r="B45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" t="s">
-        <v>173</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="B45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E45" t="s">
-        <v>155</v>
+      <c r="E45" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="H45">
         <v>34</v>
@@ -2325,24 +2590,24 @@
         <v>Tu veux qu'un copain t'accompagne?</v>
       </c>
       <c r="J45" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46">
+      <c r="A46" s="2">
         <v>44</v>
       </c>
-      <c r="B46" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" t="s">
-        <v>173</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="B46" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E46" t="s">
-        <v>156</v>
+      <c r="E46" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="H46">
         <v>35</v>
@@ -2352,24 +2617,24 @@
         <v>C'est pas grave</v>
       </c>
       <c r="J46" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47">
+      <c r="A47" s="2">
         <v>45</v>
       </c>
-      <c r="B47" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" t="s">
-        <v>173</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="B47" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E47" t="s">
-        <v>157</v>
+      <c r="E47" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="H47">
         <v>35</v>
@@ -2383,20 +2648,20 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48">
+      <c r="A48" s="2">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" t="s">
-        <v>173</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="B48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E48" t="s">
-        <v>158</v>
+      <c r="E48" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="H48">
         <v>36</v>
@@ -2406,24 +2671,24 @@
         <v>On va te trouver des nouveaux vêtements</v>
       </c>
       <c r="J48" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="A49" s="2">
         <v>47</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C49" t="s">
-        <v>173</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="C49" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E49" t="s">
-        <v>159</v>
+      <c r="E49" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="H49">
         <v>37</v>
@@ -2437,20 +2702,20 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="A50" s="2">
         <v>48</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C50" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="C50" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E50" t="s">
-        <v>160</v>
+      <c r="E50" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="H50">
         <v>38</v>
@@ -2460,24 +2725,24 @@
         <v>Tu n'as pas compris ce qu'il fallait faire?</v>
       </c>
       <c r="J50" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="A51" s="2">
         <v>49</v>
       </c>
-      <c r="B51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" t="s">
-        <v>173</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="B51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E51" t="s">
-        <v>161</v>
+      <c r="E51" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="H51">
         <v>39</v>
@@ -2491,20 +2756,20 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52">
+      <c r="A52" s="2">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
-        <v>4</v>
-      </c>
-      <c r="C52" t="s">
-        <v>174</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="B52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E52" t="s">
-        <v>162</v>
+      <c r="E52" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="H52">
         <v>40</v>
@@ -2518,20 +2783,20 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53">
+      <c r="A53" s="2">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C53" t="s">
-        <v>174</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="C53" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E53" t="s">
-        <v>163</v>
+      <c r="E53" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="H53">
         <v>41</v>
@@ -2545,20 +2810,20 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="A54" s="2">
         <v>52</v>
       </c>
-      <c r="B54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" t="s">
-        <v>174</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="B54" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E54" t="s">
-        <v>164</v>
+      <c r="E54" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="H54">
         <v>41</v>
@@ -2572,20 +2837,20 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A55">
+      <c r="A55" s="2">
         <v>53</v>
       </c>
-      <c r="B55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55" t="s">
-        <v>174</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="B55" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E55" t="s">
-        <v>165</v>
+      <c r="E55" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="H55">
         <v>42</v>
@@ -2599,20 +2864,20 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="A56" s="2">
         <v>54</v>
       </c>
-      <c r="B56" t="s">
-        <v>4</v>
-      </c>
-      <c r="C56" t="s">
-        <v>174</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="B56" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E56" t="s">
-        <v>166</v>
+      <c r="E56" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="H56">
         <v>43</v>
@@ -2626,20 +2891,20 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57">
+      <c r="A57" s="2">
         <v>55</v>
       </c>
-      <c r="B57" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" t="s">
-        <v>174</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="B57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E57" t="s">
-        <v>167</v>
+      <c r="E57" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="H57">
         <v>44</v>
@@ -2653,20 +2918,20 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58">
+      <c r="A58" s="2">
         <v>56</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C58" t="s">
-        <v>174</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="C58" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E58" t="s">
-        <v>168</v>
+      <c r="E58" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="H58">
         <v>45</v>
@@ -2680,17 +2945,20 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59">
+      <c r="A59" s="2">
         <v>57</v>
       </c>
-      <c r="B59" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59" t="s">
-        <v>177</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="B59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>175</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="H59">
         <v>45</v>
@@ -2700,21 +2968,24 @@
         <v>Tu as oublié tes affaires de gym?</v>
       </c>
       <c r="J59" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60">
+      <c r="A60" s="2">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" t="s">
-        <v>177</v>
-      </c>
-      <c r="D60" t="s">
-        <v>176</v>
+      <c r="B60" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="H60">
         <v>46</v>
@@ -2728,17 +2999,20 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A61">
+      <c r="A61" s="2">
         <v>59</v>
       </c>
-      <c r="B61" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" t="s">
-        <v>177</v>
-      </c>
-      <c r="D61" t="s">
-        <v>178</v>
+      <c r="B61" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="H61">
         <v>47</v>
@@ -2748,21 +3022,24 @@
         <v>Je vais t'en prêter</v>
       </c>
       <c r="J61" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A62">
+      <c r="A62" s="2">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" t="s">
-        <v>169</v>
-      </c>
-      <c r="D62" t="s">
-        <v>179</v>
+      <c r="B62" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>231</v>
       </c>
       <c r="H62">
         <v>47</v>
@@ -2772,21 +3049,24 @@
         <v>Je vais t'en prêter</v>
       </c>
       <c r="J62" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A63">
+      <c r="A63" s="2">
         <v>61</v>
       </c>
-      <c r="B63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" t="s">
-        <v>173</v>
-      </c>
-      <c r="D63" t="s">
-        <v>180</v>
+      <c r="B63" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="H63">
         <v>48</v>
@@ -2800,17 +3080,20 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64">
+      <c r="A64" s="2">
         <v>62</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C64" t="s">
-        <v>171</v>
-      </c>
-      <c r="D64" t="s">
-        <v>181</v>
+      <c r="C64" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>227</v>
       </c>
       <c r="H64">
         <v>49</v>
@@ -2824,17 +3107,20 @@
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65">
+      <c r="A65" s="2">
         <v>63</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C65" t="s">
-        <v>169</v>
-      </c>
-      <c r="D65" t="s">
-        <v>182</v>
+      <c r="C65" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="H65">
         <v>50</v>
@@ -2848,17 +3134,20 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66">
+      <c r="A66" s="4">
         <v>64</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C66" t="s">
-        <v>169</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>183</v>
+      <c r="C66" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>228</v>
       </c>
       <c r="H66">
         <v>50</v>
@@ -2872,6 +3161,21 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="4">
+        <v>65</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>215</v>
+      </c>
       <c r="H67">
         <v>51</v>
       </c>
@@ -2880,10 +3184,25 @@
         <v>Ne t'inquiète pas.</v>
       </c>
       <c r="J67" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="4">
+        <v>66</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>229</v>
+      </c>
       <c r="H68">
         <v>52</v>
       </c>
@@ -2896,6 +3215,11 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
       <c r="H69">
         <v>53</v>
       </c>
@@ -2940,7 +3264,7 @@
         <v>Tu les retrouveras tout bientôt.</v>
       </c>
       <c r="J72" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
@@ -2952,7 +3276,7 @@
         <v>Es-tu en colère?</v>
       </c>
       <c r="J73" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
@@ -2964,7 +3288,7 @@
         <v>As-tu peur?</v>
       </c>
       <c r="J74" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
@@ -2976,7 +3300,7 @@
         <v>As-tu peur?</v>
       </c>
       <c r="J75" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
@@ -2988,7 +3312,7 @@
         <v>Es-tu triste?</v>
       </c>
       <c r="J76" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
@@ -2997,10 +3321,10 @@
       </c>
       <c r="I77" t="str">
         <f>VLOOKUP(H77,source[],4)</f>
-        <v>As-tu des démangeaisons ?</v>
+        <v>Ça te gratte quelque part?</v>
       </c>
       <c r="J77" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
@@ -3009,10 +3333,10 @@
       </c>
       <c r="I78" t="str">
         <f>VLOOKUP(H78,source[],4)</f>
-        <v>As-tu des démangeaisons ?</v>
+        <v>Ça te gratte quelque part?</v>
       </c>
       <c r="J78" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
@@ -3024,7 +3348,7 @@
         <v>As-tu perdu quelque chose ?</v>
       </c>
       <c r="J79" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
@@ -3036,7 +3360,7 @@
         <v>On va nettoyer ça, ne t’inquiète pas.</v>
       </c>
       <c r="J80" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="81" spans="8:10" x14ac:dyDescent="0.3">
@@ -3048,7 +3372,79 @@
         <v>Respire calmement, ça va passer.</v>
       </c>
       <c r="J81" t="s">
-        <v>210</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="82" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H82">
+        <v>64</v>
+      </c>
+      <c r="I82" t="str">
+        <f>VLOOKUP(H82,source[],4)</f>
+        <v>Il faut que tu boives quelque chose</v>
+      </c>
+      <c r="J82" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="83" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H83">
+        <v>64</v>
+      </c>
+      <c r="I83" t="str">
+        <f>VLOOKUP(H83,source[],4)</f>
+        <v>Il faut que tu boives quelque chose</v>
+      </c>
+      <c r="J83" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="84" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H84">
+        <v>65</v>
+      </c>
+      <c r="I84" t="str">
+        <f>VLOOKUP(H84,source[],4)</f>
+        <v>Tu as perdu quelque chose?</v>
+      </c>
+      <c r="J84" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="85" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H85">
+        <v>65</v>
+      </c>
+      <c r="I85" t="str">
+        <f>VLOOKUP(H85,source[],4)</f>
+        <v>Tu as perdu quelque chose?</v>
+      </c>
+      <c r="J85" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="86" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H86">
+        <v>66</v>
+      </c>
+      <c r="I86" t="str">
+        <f>VLOOKUP(H86,source[],4)</f>
+        <v>Tu veux me montrer quelque chose?</v>
+      </c>
+      <c r="J86" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="87" spans="8:10" x14ac:dyDescent="0.3">
+      <c r="H87">
+        <v>66</v>
+      </c>
+      <c r="I87" t="str">
+        <f>VLOOKUP(H87,source[],4)</f>
+        <v>Tu veux me montrer quelque chose?</v>
+      </c>
+      <c r="J87" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3061,23 +3457,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5e3a48d8-7e97-4140-96a4-9af8ed81797d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D0C1FCA18A99D34AAFDDFF46DD1E91A1" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e541d088f59b4fc9f823a894c4e813a1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5e3a48d8-7e97-4140-96a4-9af8ed81797d" xmlns:ns4="5f85ec69-15ba-4716-b649-82af49937962" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="291725a629dd727e9cbbb438f4c55961" ns3:_="" ns4:_="">
     <xsd:import namespace="5e3a48d8-7e97-4140-96a4-9af8ed81797d"/>
@@ -3298,40 +3677,33 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0838CF8F-8378-4A1D-A58E-CCAEB0AEECC0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5e3a48d8-7e97-4140-96a4-9af8ed81797d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19E1176B-FD25-4DCF-A2F3-AB362754F51C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5e3a48d8-7e97-4140-96a4-9af8ed81797d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5f85ec69-15ba-4716-b649-82af49937962"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1210E72-E394-4977-A48D-DF6B50442432}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="5e3a48d8-7e97-4140-96a4-9af8ed81797d"/>
     <ds:schemaRef ds:uri="5f85ec69-15ba-4716-b649-82af49937962"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -3340,4 +3712,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19E1176B-FD25-4DCF-A2F3-AB362754F51C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
+    <ds:schemaRef ds:uri="5e3a48d8-7e97-4140-96a4-9af8ed81797d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema-instance"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0838CF8F-8378-4A1D-A58E-CCAEB0AEECC0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>